<commit_message>
scenes depth maps complete
</commit_message>
<xml_diff>
--- a/Stimuli/Images/DepthMaps/depths.xlsx
+++ b/Stimuli/Images/DepthMaps/depths.xlsx
@@ -8,15 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Becca\Documents\GitHub\fMRI_ef_scrambled-objects_2022\Stimuli\Images\DepthMaps\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{004F7881-D280-426C-9F2F-F7352D9069C1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D596376E-F2E6-4F69-82D9-AC285FF5CC1B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="14400" yWindow="0" windowWidth="14400" windowHeight="15600" xr2:uid="{A60B6263-5EC6-4E52-B93A-1BC494533CA5}"/>
+    <workbookView xWindow="-16320" yWindow="-9420" windowWidth="16440" windowHeight="28440" xr2:uid="{A60B6263-5EC6-4E52-B93A-1BC494533CA5}"/>
   </bookViews>
   <sheets>
     <sheet name="Stimulus" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="191029"/>
-  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -37,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="105" uniqueCount="93">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="184" uniqueCount="141">
   <si>
     <t>apple</t>
   </si>
@@ -316,13 +315,180 @@
   </si>
   <si>
     <t>Blender 2, base body 12</t>
+  </si>
+  <si>
+    <t>object-solid_07</t>
+  </si>
+  <si>
+    <t>object-solid_01</t>
+  </si>
+  <si>
+    <t>object-solid_02</t>
+  </si>
+  <si>
+    <t>object-solid_03</t>
+  </si>
+  <si>
+    <t>object-solid_04</t>
+  </si>
+  <si>
+    <t>object-solid_06</t>
+  </si>
+  <si>
+    <t>object-solid_08</t>
+  </si>
+  <si>
+    <t>object-solid_09</t>
+  </si>
+  <si>
+    <t>object-solid_11</t>
+  </si>
+  <si>
+    <t>object-solid_14</t>
+  </si>
+  <si>
+    <t>object-solid_16</t>
+  </si>
+  <si>
+    <t>object-solid_19</t>
+  </si>
+  <si>
+    <t>object-solid_17</t>
+  </si>
+  <si>
+    <t>object-solid_20</t>
+  </si>
+  <si>
+    <t>VX - object-solid_10</t>
+  </si>
+  <si>
+    <t>VX - object-solid_05</t>
+  </si>
+  <si>
+    <t>VX - object-solid_12</t>
+  </si>
+  <si>
+    <t>VX - object-solid_15</t>
+  </si>
+  <si>
+    <t>VX - object-solid_18</t>
+  </si>
+  <si>
+    <t>VX - object-solid_13</t>
+  </si>
+  <si>
+    <t>not used anymore</t>
+  </si>
+  <si>
+    <t xml:space="preserve">tiny &amp; flat, rotate and slant in depth? </t>
+  </si>
+  <si>
+    <t>ok, not enough depth</t>
+  </si>
+  <si>
+    <t>ok,  rotate</t>
+  </si>
+  <si>
+    <t>needs to be rotated</t>
+  </si>
+  <si>
+    <t>good, rotate  to add depth</t>
+  </si>
+  <si>
+    <t xml:space="preserve">measure </t>
+  </si>
+  <si>
+    <t>good but also needs to be rotated a bit</t>
+  </si>
+  <si>
+    <t>good depth - add texture to pot</t>
+  </si>
+  <si>
+    <t>good depth, too small, scale up a bit</t>
+  </si>
+  <si>
+    <t>bit flat looking, tiny rotation?</t>
+  </si>
+  <si>
+    <t>good could be rotated to add a bit more depth</t>
+  </si>
+  <si>
+    <t>good</t>
+  </si>
+  <si>
+    <t>rotate to increase depth otherwise good</t>
+  </si>
+  <si>
+    <t>shallow depth, needs texture on surface - not sure why the depth map values are so high - please verify</t>
+  </si>
+  <si>
+    <t>looks like a broken finger - I'd omit</t>
+  </si>
+  <si>
+    <t>too flat  - rotate?</t>
+  </si>
+  <si>
+    <t>too compact, not enough variation - omit?</t>
+  </si>
+  <si>
+    <t>too flat  - omit</t>
+  </si>
+  <si>
+    <t>check this one - the depth differencce is high but it looks flat- rotate?</t>
+  </si>
+  <si>
+    <t>odd angle - either rotate or omit?</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Aim for  150 +- 2cm? - for objects &amp; body parts? Depending on feasiblity, could aim for 200 - that would bring them closer to the faces.  </t>
+  </si>
+  <si>
+    <t>Laurie feedback</t>
+  </si>
+  <si>
+    <t xml:space="preserve">too small - remove? </t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">there were two of these - I used the one </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>without</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> _v1</t>
+    </r>
+  </si>
+  <si>
+    <t>Cannot rescale the faces (orthostereopsis) but need to make sure 1. they are all positioned with the nasion at screen plane 2. drop extreme faces (&lt; 225 and &gt; 299 ?)</t>
+  </si>
+  <si>
+    <t>only version had _v1 - is this the correct one? Unsure why the disp diff is so large - is that correct? If so scale down or omit</t>
+  </si>
+  <si>
+    <t xml:space="preserve">*male 14 could be used instead of  other if needed. </t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="7">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -344,6 +510,32 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFC00000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFC00000"/>
+      <name val="Calibri (Body)"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="4"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -353,7 +545,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="12">
+  <borders count="13">
     <border>
       <left/>
       <right/>
@@ -478,11 +670,26 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="20">
+  <cellXfs count="43">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
@@ -502,12 +709,35 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="22">
+  <dxfs count="23">
     <dxf>
       <numFmt numFmtId="0" formatCode="General"/>
     </dxf>
@@ -690,6 +920,18 @@
       </font>
     </dxf>
     <dxf>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right/>
+        <top/>
+        <bottom/>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
       <numFmt numFmtId="0" formatCode="General"/>
       <border diagonalUp="0" diagonalDown="0">
         <left style="thin">
@@ -760,13 +1002,14 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{3A449E8A-54D5-4F96-B244-604FFA469FAB}" name="Table1" displayName="Table1" ref="A1:D23" totalsRowShown="0" headerRowDxfId="21">
-  <autoFilter ref="A1:D23" xr:uid="{3A449E8A-54D5-4F96-B244-604FFA469FAB}"/>
-  <tableColumns count="4">
-    <tableColumn id="1" xr3:uid="{55B9CB86-FFCE-4001-84E7-926E143A4754}" name="Object" dataDxfId="20"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{3A449E8A-54D5-4F96-B244-604FFA469FAB}" name="Table1" displayName="Table1" ref="A1:E23" totalsRowShown="0" headerRowDxfId="22">
+  <autoFilter ref="A1:E23" xr:uid="{3A449E8A-54D5-4F96-B244-604FFA469FAB}"/>
+  <tableColumns count="5">
+    <tableColumn id="1" xr3:uid="{55B9CB86-FFCE-4001-84E7-926E143A4754}" name="Object" dataDxfId="21"/>
     <tableColumn id="2" xr3:uid="{154C99C7-865E-4E8A-A7F6-E66DA111723A}" name="min (mm)"/>
-    <tableColumn id="3" xr3:uid="{AE9CF431-6E41-4056-8560-A1AC568C7EBE}" name="max (mm)" dataDxfId="19"/>
-    <tableColumn id="5" xr3:uid="{76DFDC72-E303-4FEC-BA19-A7B7905D48E6}" name="difference" dataDxfId="18"/>
+    <tableColumn id="3" xr3:uid="{AE9CF431-6E41-4056-8560-A1AC568C7EBE}" name="max (mm)" dataDxfId="20"/>
+    <tableColumn id="5" xr3:uid="{76DFDC72-E303-4FEC-BA19-A7B7905D48E6}" name="difference" dataDxfId="19"/>
+    <tableColumn id="4" xr3:uid="{86CCC425-700A-4799-9101-C4A00D694DF1}" name="Name for Laurie" dataDxfId="18"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium18" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1130,13 +1373,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{305C46E9-DBCF-4732-A226-FBA3B04D35E8}">
-  <dimension ref="A1:E114"/>
+  <dimension ref="A1:O114"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G29" sqref="G29"/>
+      <selection activeCell="K77" sqref="K77"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="21.7109375" customWidth="1"/>
     <col min="2" max="3" width="11" customWidth="1"/>
@@ -1144,7 +1387,7 @@
     <col min="5" max="5" width="16.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:15">
       <c r="A1" s="15" t="s">
         <v>25</v>
       </c>
@@ -1157,9 +1400,28 @@
       <c r="D1" s="10" t="s">
         <v>24</v>
       </c>
-      <c r="E1" s="6"/>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E1" s="12" t="s">
+        <v>71</v>
+      </c>
+      <c r="I1" s="30" t="s">
+        <v>25</v>
+      </c>
+      <c r="J1" s="31" t="s">
+        <v>23</v>
+      </c>
+      <c r="K1" s="27" t="s">
+        <v>22</v>
+      </c>
+      <c r="L1" s="26" t="s">
+        <v>24</v>
+      </c>
+      <c r="M1" s="28"/>
+      <c r="N1" s="29" t="s">
+        <v>135</v>
+      </c>
+      <c r="O1" s="29"/>
+    </row>
+    <row r="2" spans="1:15">
       <c r="A2" s="17" t="s">
         <v>0</v>
       </c>
@@ -1172,9 +1434,30 @@
       <c r="D2" s="6">
         <v>96.424999999999997</v>
       </c>
-      <c r="E2" s="6"/>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E2" s="6" t="s">
+        <v>93</v>
+      </c>
+      <c r="I2" s="32" t="s">
+        <v>11</v>
+      </c>
+      <c r="J2" s="20">
+        <v>7.3550000000000004</v>
+      </c>
+      <c r="K2" s="21">
+        <v>46.506</v>
+      </c>
+      <c r="L2" s="22">
+        <v>39.151000000000003</v>
+      </c>
+      <c r="M2" s="22">
+        <v>16</v>
+      </c>
+      <c r="N2" s="20" t="s">
+        <v>114</v>
+      </c>
+      <c r="O2" s="20"/>
+    </row>
+    <row r="3" spans="1:15">
       <c r="A3" s="17" t="s">
         <v>1</v>
       </c>
@@ -1187,9 +1470,30 @@
       <c r="D3" s="6">
         <v>44.561999999999998</v>
       </c>
-      <c r="E3" s="6"/>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E3" s="6" t="s">
+        <v>94</v>
+      </c>
+      <c r="I3" s="32" t="s">
+        <v>1</v>
+      </c>
+      <c r="J3" s="20">
+        <v>4.6399999999999997</v>
+      </c>
+      <c r="K3" s="21">
+        <v>49.201999999999998</v>
+      </c>
+      <c r="L3" s="22">
+        <v>44.561999999999998</v>
+      </c>
+      <c r="M3" s="22">
+        <v>1</v>
+      </c>
+      <c r="N3" s="20" t="s">
+        <v>115</v>
+      </c>
+      <c r="O3" s="20"/>
+    </row>
+    <row r="4" spans="1:15">
       <c r="A4" s="17" t="s">
         <v>2</v>
       </c>
@@ -1202,9 +1506,30 @@
       <c r="D4" s="6">
         <v>104.587</v>
       </c>
-      <c r="E4" s="6"/>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E4" s="6" t="s">
+        <v>95</v>
+      </c>
+      <c r="I4" s="32" t="s">
+        <v>17</v>
+      </c>
+      <c r="J4" s="20">
+        <v>7.7069999999999999</v>
+      </c>
+      <c r="K4" s="21">
+        <v>56.966999999999999</v>
+      </c>
+      <c r="L4" s="22">
+        <v>49.26</v>
+      </c>
+      <c r="M4" s="22">
+        <v>19</v>
+      </c>
+      <c r="N4" s="20" t="s">
+        <v>116</v>
+      </c>
+      <c r="O4" s="20"/>
+    </row>
+    <row r="5" spans="1:15">
       <c r="A5" s="17" t="s">
         <v>3</v>
       </c>
@@ -1217,9 +1542,30 @@
       <c r="D5" s="6">
         <v>61.048000000000002</v>
       </c>
-      <c r="E5" s="6"/>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E5" s="6" t="s">
+        <v>96</v>
+      </c>
+      <c r="I5" s="34" t="s">
+        <v>7</v>
+      </c>
+      <c r="J5" s="20">
+        <v>11.573</v>
+      </c>
+      <c r="K5" s="21">
+        <v>72.433000000000007</v>
+      </c>
+      <c r="L5" s="22">
+        <v>60.86</v>
+      </c>
+      <c r="M5" s="22">
+        <v>10</v>
+      </c>
+      <c r="N5" s="20" t="s">
+        <v>117</v>
+      </c>
+      <c r="O5" s="20"/>
+    </row>
+    <row r="6" spans="1:15">
       <c r="A6" s="17" t="s">
         <v>4</v>
       </c>
@@ -1232,9 +1578,30 @@
       <c r="D6" s="6">
         <v>109.76900000000001</v>
       </c>
-      <c r="E6" s="6"/>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E6" s="6" t="s">
+        <v>97</v>
+      </c>
+      <c r="I6" s="20" t="s">
+        <v>3</v>
+      </c>
+      <c r="J6" s="20">
+        <v>23.443000000000001</v>
+      </c>
+      <c r="K6" s="20">
+        <v>84.491</v>
+      </c>
+      <c r="L6" s="20">
+        <v>61.048000000000002</v>
+      </c>
+      <c r="M6" s="20">
+        <v>3</v>
+      </c>
+      <c r="N6" s="20" t="s">
+        <v>118</v>
+      </c>
+      <c r="O6" s="20"/>
+    </row>
+    <row r="7" spans="1:15">
       <c r="A7" s="17" t="s">
         <v>20</v>
       </c>
@@ -1247,9 +1614,33 @@
       <c r="D7" s="6">
         <v>57.819000000000003</v>
       </c>
-      <c r="E7" s="6"/>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E7" s="6" t="s">
+        <v>108</v>
+      </c>
+      <c r="F7" t="s">
+        <v>113</v>
+      </c>
+      <c r="I7" s="35" t="s">
+        <v>119</v>
+      </c>
+      <c r="J7" s="20">
+        <v>13.423999999999999</v>
+      </c>
+      <c r="K7" s="21">
+        <v>101.03</v>
+      </c>
+      <c r="L7" s="22">
+        <v>87.605999999999995</v>
+      </c>
+      <c r="M7" s="22">
+        <v>12</v>
+      </c>
+      <c r="N7" s="20" t="s">
+        <v>120</v>
+      </c>
+      <c r="O7" s="20"/>
+    </row>
+    <row r="8" spans="1:15">
       <c r="A8" s="17" t="s">
         <v>5</v>
       </c>
@@ -1262,9 +1653,30 @@
       <c r="D8" s="6">
         <v>100.39400000000001</v>
       </c>
-      <c r="E8" s="6"/>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E8" s="6" t="s">
+        <v>98</v>
+      </c>
+      <c r="I8" s="32" t="s">
+        <v>10</v>
+      </c>
+      <c r="J8" s="20">
+        <v>-0.75900000000000001</v>
+      </c>
+      <c r="K8" s="21">
+        <v>90.295000000000002</v>
+      </c>
+      <c r="L8" s="22">
+        <v>91.054000000000002</v>
+      </c>
+      <c r="M8" s="22">
+        <v>14</v>
+      </c>
+      <c r="N8" s="20" t="s">
+        <v>121</v>
+      </c>
+      <c r="O8" s="20"/>
+    </row>
+    <row r="9" spans="1:15">
       <c r="A9" s="17" t="s">
         <v>6</v>
       </c>
@@ -1277,9 +1689,30 @@
       <c r="D9" s="6">
         <v>115.7158</v>
       </c>
-      <c r="E9" s="6"/>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E9" s="6" t="s">
+        <v>99</v>
+      </c>
+      <c r="I9" s="32" t="s">
+        <v>0</v>
+      </c>
+      <c r="J9" s="20">
+        <v>0.42399999999999999</v>
+      </c>
+      <c r="K9" s="21">
+        <v>96.849000000000004</v>
+      </c>
+      <c r="L9" s="22">
+        <v>96.424999999999997</v>
+      </c>
+      <c r="M9" s="22">
+        <v>7</v>
+      </c>
+      <c r="N9" s="20" t="s">
+        <v>122</v>
+      </c>
+      <c r="O9" s="20"/>
+    </row>
+    <row r="10" spans="1:15">
       <c r="A10" s="17" t="s">
         <v>21</v>
       </c>
@@ -1292,9 +1725,30 @@
       <c r="D10" s="6">
         <v>109.5731</v>
       </c>
-      <c r="E10" s="6"/>
-    </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E10" s="6" t="s">
+        <v>100</v>
+      </c>
+      <c r="I10" s="32" t="s">
+        <v>5</v>
+      </c>
+      <c r="J10" s="20">
+        <v>0.86599999999999999</v>
+      </c>
+      <c r="K10" s="21">
+        <v>101.26</v>
+      </c>
+      <c r="L10" s="22">
+        <v>100.39400000000001</v>
+      </c>
+      <c r="M10" s="22">
+        <v>6</v>
+      </c>
+      <c r="N10" s="20" t="s">
+        <v>123</v>
+      </c>
+      <c r="O10" s="20"/>
+    </row>
+    <row r="11" spans="1:15">
       <c r="A11" s="17" t="s">
         <v>7</v>
       </c>
@@ -1307,9 +1761,33 @@
       <c r="D11" s="6">
         <v>60.86</v>
       </c>
-      <c r="E11" s="6"/>
-    </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E11" s="6" t="s">
+        <v>107</v>
+      </c>
+      <c r="F11" t="s">
+        <v>113</v>
+      </c>
+      <c r="I11" s="32" t="s">
+        <v>2</v>
+      </c>
+      <c r="J11" s="20">
+        <v>9.0129999999999999</v>
+      </c>
+      <c r="K11" s="21">
+        <v>113.6</v>
+      </c>
+      <c r="L11" s="22">
+        <v>104.587</v>
+      </c>
+      <c r="M11" s="22">
+        <v>2</v>
+      </c>
+      <c r="N11" s="20" t="s">
+        <v>124</v>
+      </c>
+      <c r="O11" s="20"/>
+    </row>
+    <row r="12" spans="1:15">
       <c r="A12" s="17" t="s">
         <v>8</v>
       </c>
@@ -1322,9 +1800,30 @@
       <c r="D12" s="6">
         <v>65.296999999999997</v>
       </c>
-      <c r="E12" s="6"/>
-    </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E12" s="6" t="s">
+        <v>101</v>
+      </c>
+      <c r="I12" s="32" t="s">
+        <v>21</v>
+      </c>
+      <c r="J12" s="20">
+        <v>1.0669</v>
+      </c>
+      <c r="K12" s="21">
+        <v>110.64</v>
+      </c>
+      <c r="L12" s="22">
+        <v>109.5731</v>
+      </c>
+      <c r="M12" s="22">
+        <v>9</v>
+      </c>
+      <c r="N12" s="20" t="s">
+        <v>125</v>
+      </c>
+      <c r="O12" s="36"/>
+    </row>
+    <row r="13" spans="1:15">
       <c r="A13" s="17" t="s">
         <v>9</v>
       </c>
@@ -1337,9 +1836,33 @@
       <c r="D13" s="6">
         <v>24.213999999999999</v>
       </c>
-      <c r="E13" s="6"/>
-    </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E13" s="6" t="s">
+        <v>112</v>
+      </c>
+      <c r="F13" t="s">
+        <v>113</v>
+      </c>
+      <c r="I13" s="32" t="s">
+        <v>4</v>
+      </c>
+      <c r="J13" s="20">
+        <v>13.301</v>
+      </c>
+      <c r="K13" s="21">
+        <v>123.07</v>
+      </c>
+      <c r="L13" s="22">
+        <v>109.76900000000001</v>
+      </c>
+      <c r="M13" s="22">
+        <v>4</v>
+      </c>
+      <c r="N13" s="20" t="s">
+        <v>126</v>
+      </c>
+      <c r="O13" s="36"/>
+    </row>
+    <row r="14" spans="1:15">
       <c r="A14" s="17" t="s">
         <v>10</v>
       </c>
@@ -1352,9 +1875,30 @@
       <c r="D14" s="6">
         <v>91.054000000000002</v>
       </c>
-      <c r="E14" s="6"/>
-    </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E14" s="6" t="s">
+        <v>102</v>
+      </c>
+      <c r="I14" s="32" t="s">
+        <v>18</v>
+      </c>
+      <c r="J14" s="20">
+        <v>6.4649999999999999</v>
+      </c>
+      <c r="K14" s="21">
+        <v>117.19</v>
+      </c>
+      <c r="L14" s="22">
+        <v>110.72499999999999</v>
+      </c>
+      <c r="M14" s="22">
+        <v>20</v>
+      </c>
+      <c r="N14" s="20" t="s">
+        <v>127</v>
+      </c>
+      <c r="O14" s="36"/>
+    </row>
+    <row r="15" spans="1:15">
       <c r="A15" s="17" t="s">
         <v>11</v>
       </c>
@@ -1367,9 +1911,30 @@
       <c r="D15" s="6">
         <v>39.151000000000003</v>
       </c>
-      <c r="E15" s="6"/>
-    </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E15" s="6" t="s">
+        <v>103</v>
+      </c>
+      <c r="I15" s="32" t="s">
+        <v>6</v>
+      </c>
+      <c r="J15" s="20">
+        <v>2.4942000000000002</v>
+      </c>
+      <c r="K15" s="21">
+        <v>118.21</v>
+      </c>
+      <c r="L15" s="22">
+        <v>115.7158</v>
+      </c>
+      <c r="M15" s="22">
+        <v>8</v>
+      </c>
+      <c r="N15" s="20" t="s">
+        <v>125</v>
+      </c>
+      <c r="O15" s="36"/>
+    </row>
+    <row r="16" spans="1:15">
       <c r="A16" s="17" t="s">
         <v>12</v>
       </c>
@@ -1382,9 +1947,33 @@
       <c r="D16" s="6">
         <v>54.86</v>
       </c>
-      <c r="E16" s="6"/>
-    </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E16" s="6" t="s">
+        <v>110</v>
+      </c>
+      <c r="F16" t="s">
+        <v>113</v>
+      </c>
+      <c r="I16" s="33" t="s">
+        <v>15</v>
+      </c>
+      <c r="J16" s="24">
+        <v>7.79</v>
+      </c>
+      <c r="K16" s="25">
+        <v>131.26</v>
+      </c>
+      <c r="L16" s="23">
+        <v>123.47</v>
+      </c>
+      <c r="M16" s="22">
+        <v>17</v>
+      </c>
+      <c r="N16" s="20" t="s">
+        <v>125</v>
+      </c>
+      <c r="O16" s="36"/>
+    </row>
+    <row r="17" spans="1:12">
       <c r="A17" s="17" t="s">
         <v>13</v>
       </c>
@@ -1399,7 +1988,7 @@
       </c>
       <c r="E17" s="6"/>
     </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:12">
       <c r="A18" s="17" t="s">
         <v>14</v>
       </c>
@@ -1412,9 +2001,14 @@
       <c r="D18" s="6">
         <v>87.605999999999995</v>
       </c>
-      <c r="E18" s="6"/>
-    </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E18" s="6" t="s">
+        <v>109</v>
+      </c>
+      <c r="F18" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="19" spans="1:12">
       <c r="A19" s="17" t="s">
         <v>15</v>
       </c>
@@ -1427,9 +2021,11 @@
       <c r="D19" s="6">
         <v>123.47</v>
       </c>
-      <c r="E19" s="6"/>
-    </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E19" s="6" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="20" spans="1:12">
       <c r="A20" s="17" t="s">
         <v>16</v>
       </c>
@@ -1442,9 +2038,14 @@
       <c r="D20" s="6">
         <v>83.828999999999994</v>
       </c>
-      <c r="E20" s="6"/>
-    </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E20" s="6" t="s">
+        <v>111</v>
+      </c>
+      <c r="F20" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="21" spans="1:12">
       <c r="A21" s="17" t="s">
         <v>17</v>
       </c>
@@ -1457,9 +2058,11 @@
       <c r="D21" s="6">
         <v>49.26</v>
       </c>
-      <c r="E21" s="6"/>
-    </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E21" s="6" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="22" spans="1:12">
       <c r="A22" s="17" t="s">
         <v>18</v>
       </c>
@@ -1472,9 +2075,11 @@
       <c r="D22" s="6">
         <v>110.72499999999999</v>
       </c>
-      <c r="E22" s="6"/>
-    </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E22" s="6" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="23" spans="1:12">
       <c r="A23" s="18" t="s">
         <v>19</v>
       </c>
@@ -1488,8 +2093,11 @@
         <v>104.876</v>
       </c>
       <c r="E23" s="6"/>
-    </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F23" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="25" spans="1:12">
       <c r="A25" s="14" t="s">
         <v>91</v>
       </c>
@@ -1505,8 +2113,11 @@
       <c r="E25" s="14" t="s">
         <v>71</v>
       </c>
-    </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="I25" s="19" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="26" spans="1:12">
       <c r="A26" t="s">
         <v>33</v>
       </c>
@@ -1523,8 +2134,14 @@
       <c r="E26" t="s">
         <v>72</v>
       </c>
-    </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="I26" s="39" t="s">
+        <v>128</v>
+      </c>
+      <c r="J26" s="37"/>
+      <c r="K26" s="37"/>
+      <c r="L26" s="37"/>
+    </row>
+    <row r="27" spans="1:12">
       <c r="A27" t="s">
         <v>32</v>
       </c>
@@ -1541,8 +2158,12 @@
       <c r="E27" t="s">
         <v>73</v>
       </c>
-    </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="I27" s="39"/>
+      <c r="J27" s="37"/>
+      <c r="K27" s="37"/>
+      <c r="L27" s="37"/>
+    </row>
+    <row r="28" spans="1:12">
       <c r="A28" t="s">
         <v>31</v>
       </c>
@@ -1559,8 +2180,12 @@
       <c r="E28" t="s">
         <v>74</v>
       </c>
-    </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="I28" s="39"/>
+      <c r="J28" s="37"/>
+      <c r="K28" s="37"/>
+      <c r="L28" s="37"/>
+    </row>
+    <row r="29" spans="1:12">
       <c r="A29" t="s">
         <v>30</v>
       </c>
@@ -1577,8 +2202,14 @@
       <c r="E29" t="s">
         <v>75</v>
       </c>
-    </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="I29" s="39" t="s">
+        <v>129</v>
+      </c>
+      <c r="J29" s="37"/>
+      <c r="K29" s="37"/>
+      <c r="L29" s="37"/>
+    </row>
+    <row r="30" spans="1:12">
       <c r="A30" t="s">
         <v>29</v>
       </c>
@@ -1595,8 +2226,12 @@
       <c r="E30" t="s">
         <v>76</v>
       </c>
-    </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="I30" s="39"/>
+      <c r="J30" s="37"/>
+      <c r="K30" s="37"/>
+      <c r="L30" s="37"/>
+    </row>
+    <row r="31" spans="1:12">
       <c r="A31" t="s">
         <v>34</v>
       </c>
@@ -1613,8 +2248,14 @@
       <c r="E31" t="s">
         <v>78</v>
       </c>
-    </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="I31" s="39" t="s">
+        <v>130</v>
+      </c>
+      <c r="J31" s="37"/>
+      <c r="K31" s="37"/>
+      <c r="L31" s="37"/>
+    </row>
+    <row r="32" spans="1:12">
       <c r="A32" t="s">
         <v>35</v>
       </c>
@@ -1631,8 +2272,12 @@
       <c r="E32" t="s">
         <v>79</v>
       </c>
-    </row>
-    <row r="33" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="I32" s="39"/>
+      <c r="J32" s="37"/>
+      <c r="K32" s="37"/>
+      <c r="L32" s="37"/>
+    </row>
+    <row r="33" spans="1:12">
       <c r="A33" t="s">
         <v>92</v>
       </c>
@@ -1642,15 +2287,21 @@
       <c r="C33" s="2">
         <v>121.87</v>
       </c>
-      <c r="D33" s="19">
+      <c r="D33">
         <f>Table5[[#This Row],[max (mm)]]-Table5[[#This Row],[min (mm)]]</f>
         <v>119.50190000000001</v>
       </c>
       <c r="E33" t="s">
         <v>77</v>
       </c>
-    </row>
-    <row r="34" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="I33" s="39" t="s">
+        <v>131</v>
+      </c>
+      <c r="J33" s="37"/>
+      <c r="K33" s="37"/>
+      <c r="L33" s="37"/>
+    </row>
+    <row r="34" spans="1:12">
       <c r="A34" t="s">
         <v>36</v>
       </c>
@@ -1667,8 +2318,12 @@
       <c r="E34" t="s">
         <v>83</v>
       </c>
-    </row>
-    <row r="35" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="I34" s="39"/>
+      <c r="J34" s="37"/>
+      <c r="K34" s="37"/>
+      <c r="L34" s="37"/>
+    </row>
+    <row r="35" spans="1:12">
       <c r="A35" t="s">
         <v>37</v>
       </c>
@@ -1685,8 +2340,12 @@
       <c r="E35" t="s">
         <v>82</v>
       </c>
-    </row>
-    <row r="36" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="I35" s="39"/>
+      <c r="J35" s="37"/>
+      <c r="K35" s="37"/>
+      <c r="L35" s="37"/>
+    </row>
+    <row r="36" spans="1:12">
       <c r="A36" t="s">
         <v>38</v>
       </c>
@@ -1703,8 +2362,12 @@
       <c r="E36" t="s">
         <v>87</v>
       </c>
-    </row>
-    <row r="37" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="I36" s="39"/>
+      <c r="J36" s="37"/>
+      <c r="K36" s="37"/>
+      <c r="L36" s="37"/>
+    </row>
+    <row r="37" spans="1:12">
       <c r="A37" t="s">
         <v>39</v>
       </c>
@@ -1721,8 +2384,14 @@
       <c r="E37" t="s">
         <v>81</v>
       </c>
-    </row>
-    <row r="38" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="I37" s="39" t="s">
+        <v>132</v>
+      </c>
+      <c r="J37" s="37"/>
+      <c r="K37" s="37"/>
+      <c r="L37" s="37"/>
+    </row>
+    <row r="38" spans="1:12">
       <c r="A38" t="s">
         <v>40</v>
       </c>
@@ -1739,8 +2408,12 @@
       <c r="E38" t="s">
         <v>86</v>
       </c>
-    </row>
-    <row r="39" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="I38" s="39"/>
+      <c r="J38" s="37"/>
+      <c r="K38" s="37"/>
+      <c r="L38" s="37"/>
+    </row>
+    <row r="39" spans="1:12">
       <c r="A39" t="s">
         <v>41</v>
       </c>
@@ -1757,8 +2430,12 @@
       <c r="E39" t="s">
         <v>85</v>
       </c>
-    </row>
-    <row r="40" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="I39" s="39"/>
+      <c r="J39" s="37"/>
+      <c r="K39" s="37"/>
+      <c r="L39" s="37"/>
+    </row>
+    <row r="40" spans="1:12">
       <c r="A40" t="s">
         <v>42</v>
       </c>
@@ -1775,8 +2452,14 @@
       <c r="E40" t="s">
         <v>84</v>
       </c>
-    </row>
-    <row r="41" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="I40" s="39" t="s">
+        <v>133</v>
+      </c>
+      <c r="J40" s="37"/>
+      <c r="K40" s="37"/>
+      <c r="L40" s="37"/>
+    </row>
+    <row r="41" spans="1:12">
       <c r="A41" t="s">
         <v>43</v>
       </c>
@@ -1793,8 +2476,12 @@
       <c r="E41" t="s">
         <v>90</v>
       </c>
-    </row>
-    <row r="42" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="I41" s="39"/>
+      <c r="J41" s="37"/>
+      <c r="K41" s="37"/>
+      <c r="L41" s="37"/>
+    </row>
+    <row r="42" spans="1:12">
       <c r="A42" t="s">
         <v>44</v>
       </c>
@@ -1811,8 +2498,12 @@
       <c r="E42" t="s">
         <v>89</v>
       </c>
-    </row>
-    <row r="43" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="I42" s="39"/>
+      <c r="J42" s="37"/>
+      <c r="K42" s="37"/>
+      <c r="L42" s="37"/>
+    </row>
+    <row r="43" spans="1:12">
       <c r="A43" t="s">
         <v>45</v>
       </c>
@@ -1829,8 +2520,12 @@
       <c r="E43" t="s">
         <v>88</v>
       </c>
-    </row>
-    <row r="44" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="I43" s="39"/>
+      <c r="J43" s="37"/>
+      <c r="K43" s="37"/>
+      <c r="L43" s="37"/>
+    </row>
+    <row r="44" spans="1:12">
       <c r="A44" t="s">
         <v>46</v>
       </c>
@@ -1847,8 +2542,14 @@
       <c r="E44" t="s">
         <v>80</v>
       </c>
-    </row>
-    <row r="46" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="I44" s="39"/>
+      <c r="J44" s="37"/>
+      <c r="K44" s="37"/>
+      <c r="L44" s="38" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="46" spans="1:12">
       <c r="A46" t="s">
         <v>26</v>
       </c>
@@ -1861,8 +2562,11 @@
       <c r="D46" s="13" t="s">
         <v>24</v>
       </c>
-    </row>
-    <row r="47" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="I46" s="19" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="47" spans="1:12">
       <c r="A47" t="s">
         <v>47</v>
       </c>
@@ -1876,8 +2580,11 @@
         <f>Table6[[#This Row],[max (mm)]]-Table6[[#This Row],[min (mm)]]</f>
         <v>278.41800000000001</v>
       </c>
-    </row>
-    <row r="48" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="I47" s="39" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="48" spans="1:12">
       <c r="A48" t="s">
         <v>48</v>
       </c>
@@ -1891,8 +2598,11 @@
         <f>Table6[[#This Row],[max (mm)]]-Table6[[#This Row],[min (mm)]]</f>
         <v>268.15107</v>
       </c>
-    </row>
-    <row r="49" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="I48" s="39" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="49" spans="1:12">
       <c r="A49" t="s">
         <v>49</v>
       </c>
@@ -1906,8 +2616,11 @@
         <f>Table6[[#This Row],[max (mm)]]-Table6[[#This Row],[min (mm)]]</f>
         <v>224.84959999999998</v>
       </c>
-    </row>
-    <row r="50" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="I49" s="39" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="50" spans="1:12">
       <c r="A50" t="s">
         <v>50</v>
       </c>
@@ -1921,8 +2634,11 @@
         <f>Table6[[#This Row],[max (mm)]]-Table6[[#This Row],[min (mm)]]</f>
         <v>264.93900000000002</v>
       </c>
-    </row>
-    <row r="51" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="I50" s="39" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="51" spans="1:12">
       <c r="A51" t="s">
         <v>51</v>
       </c>
@@ -1936,8 +2652,9 @@
         <f>Table6[[#This Row],[max (mm)]]-Table6[[#This Row],[min (mm)]]</f>
         <v>265.06</v>
       </c>
-    </row>
-    <row r="52" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="I51" s="39"/>
+    </row>
+    <row r="52" spans="1:12">
       <c r="A52" t="s">
         <v>52</v>
       </c>
@@ -1951,8 +2668,9 @@
         <f>Table6[[#This Row],[max (mm)]]-Table6[[#This Row],[min (mm)]]</f>
         <v>298.935</v>
       </c>
-    </row>
-    <row r="53" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="I52" s="39"/>
+    </row>
+    <row r="53" spans="1:12">
       <c r="A53" t="s">
         <v>53</v>
       </c>
@@ -1966,8 +2684,9 @@
         <f>Table6[[#This Row],[max (mm)]]-Table6[[#This Row],[min (mm)]]</f>
         <v>209.99900000000002</v>
       </c>
-    </row>
-    <row r="54" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="I53" s="39"/>
+    </row>
+    <row r="54" spans="1:12">
       <c r="A54" t="s">
         <v>54</v>
       </c>
@@ -1981,8 +2700,9 @@
         <f>Table6[[#This Row],[max (mm)]]-Table6[[#This Row],[min (mm)]]</f>
         <v>273.97229999999996</v>
       </c>
-    </row>
-    <row r="55" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="I54" s="39"/>
+    </row>
+    <row r="55" spans="1:12">
       <c r="A55" t="s">
         <v>55</v>
       </c>
@@ -1996,8 +2716,9 @@
         <f>Table6[[#This Row],[max (mm)]]-Table6[[#This Row],[min (mm)]]</f>
         <v>237.76599999999996</v>
       </c>
-    </row>
-    <row r="56" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="I55" s="39"/>
+    </row>
+    <row r="56" spans="1:12">
       <c r="A56" t="s">
         <v>56</v>
       </c>
@@ -2011,8 +2732,9 @@
         <f>Table6[[#This Row],[max (mm)]]-Table6[[#This Row],[min (mm)]]</f>
         <v>332.42449999999997</v>
       </c>
-    </row>
-    <row r="57" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="I56" s="39"/>
+    </row>
+    <row r="57" spans="1:12">
       <c r="A57" t="s">
         <v>57</v>
       </c>
@@ -2026,8 +2748,9 @@
         <f>Table6[[#This Row],[max (mm)]]-Table6[[#This Row],[min (mm)]]</f>
         <v>269.47039999999998</v>
       </c>
-    </row>
-    <row r="58" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="I57" s="39"/>
+    </row>
+    <row r="58" spans="1:12">
       <c r="A58" t="s">
         <v>58</v>
       </c>
@@ -2041,8 +2764,9 @@
         <f>Table6[[#This Row],[max (mm)]]-Table6[[#This Row],[min (mm)]]</f>
         <v>344.05059999999997</v>
       </c>
-    </row>
-    <row r="59" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="I58" s="39"/>
+    </row>
+    <row r="59" spans="1:12">
       <c r="A59" t="s">
         <v>59</v>
       </c>
@@ -2056,8 +2780,9 @@
         <f>Table6[[#This Row],[max (mm)]]-Table6[[#This Row],[min (mm)]]</f>
         <v>235.239</v>
       </c>
-    </row>
-    <row r="60" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="I59" s="39"/>
+    </row>
+    <row r="60" spans="1:12">
       <c r="A60" t="s">
         <v>60</v>
       </c>
@@ -2071,8 +2796,9 @@
         <f>Table6[[#This Row],[max (mm)]]-Table6[[#This Row],[min (mm)]]</f>
         <v>233.15359000000001</v>
       </c>
-    </row>
-    <row r="61" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="I60" s="39"/>
+    </row>
+    <row r="61" spans="1:12">
       <c r="A61" t="s">
         <v>61</v>
       </c>
@@ -2086,8 +2812,9 @@
         <f>Table6[[#This Row],[max (mm)]]-Table6[[#This Row],[min (mm)]]</f>
         <v>264.81900000000002</v>
       </c>
-    </row>
-    <row r="62" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="I61" s="39"/>
+    </row>
+    <row r="62" spans="1:12">
       <c r="A62" t="s">
         <v>62</v>
       </c>
@@ -2101,8 +2828,12 @@
         <f>Table6[[#This Row],[max (mm)]]-Table6[[#This Row],[min (mm)]]</f>
         <v>217.74799999999999</v>
       </c>
-    </row>
-    <row r="63" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="I62" s="39"/>
+      <c r="J62" s="40"/>
+      <c r="K62" s="40"/>
+      <c r="L62" s="40"/>
+    </row>
+    <row r="63" spans="1:12">
       <c r="A63" t="s">
         <v>63</v>
       </c>
@@ -2116,8 +2847,12 @@
         <f>Table6[[#This Row],[max (mm)]]-Table6[[#This Row],[min (mm)]]</f>
         <v>235.226</v>
       </c>
-    </row>
-    <row r="64" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="I63" s="39"/>
+      <c r="J63" s="40"/>
+      <c r="K63" s="40"/>
+      <c r="L63" s="40"/>
+    </row>
+    <row r="64" spans="1:12">
       <c r="A64" t="s">
         <v>64</v>
       </c>
@@ -2131,8 +2866,12 @@
         <f>Table6[[#This Row],[max (mm)]]-Table6[[#This Row],[min (mm)]]</f>
         <v>262.97699999999998</v>
       </c>
-    </row>
-    <row r="65" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="I64" s="39"/>
+      <c r="J64" s="40"/>
+      <c r="K64" s="40"/>
+      <c r="L64" s="40"/>
+    </row>
+    <row r="65" spans="1:12">
       <c r="A65" t="s">
         <v>65</v>
       </c>
@@ -2146,8 +2885,14 @@
         <f>Table6[[#This Row],[max (mm)]]-Table6[[#This Row],[min (mm)]]</f>
         <v>273.16000000000003</v>
       </c>
-    </row>
-    <row r="66" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="I65" s="39"/>
+      <c r="J65" s="40"/>
+      <c r="K65" s="40"/>
+      <c r="L65" s="41" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="66" spans="1:12">
       <c r="A66" t="s">
         <v>66</v>
       </c>
@@ -2161,8 +2906,12 @@
         <f>Table6[[#This Row],[max (mm)]]-Table6[[#This Row],[min (mm)]]</f>
         <v>259.56799999999998</v>
       </c>
-    </row>
-    <row r="67" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="I66" s="39"/>
+      <c r="J66" s="40"/>
+      <c r="K66" s="40"/>
+      <c r="L66" s="40"/>
+    </row>
+    <row r="67" spans="1:12">
       <c r="A67" t="s">
         <v>67</v>
       </c>
@@ -2176,8 +2925,12 @@
         <f>Table6[[#This Row],[max (mm)]]-Table6[[#This Row],[min (mm)]]</f>
         <v>226.33850000000001</v>
       </c>
-    </row>
-    <row r="68" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="I67" s="39"/>
+      <c r="J67" s="40"/>
+      <c r="K67" s="40"/>
+      <c r="L67" s="40"/>
+    </row>
+    <row r="68" spans="1:12">
       <c r="A68" t="s">
         <v>68</v>
       </c>
@@ -2191,8 +2944,12 @@
         <f>Table6[[#This Row],[max (mm)]]-Table6[[#This Row],[min (mm)]]</f>
         <v>279.27710000000002</v>
       </c>
-    </row>
-    <row r="69" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="I68" s="39"/>
+      <c r="J68" s="40"/>
+      <c r="K68" s="40"/>
+      <c r="L68" s="40"/>
+    </row>
+    <row r="69" spans="1:12">
       <c r="A69" t="s">
         <v>69</v>
       </c>
@@ -2206,8 +2963,12 @@
         <f>Table6[[#This Row],[max (mm)]]-Table6[[#This Row],[min (mm)]]</f>
         <v>237.69900000000001</v>
       </c>
-    </row>
-    <row r="70" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="I69" s="39"/>
+      <c r="J69" s="40"/>
+      <c r="K69" s="40"/>
+      <c r="L69" s="40"/>
+    </row>
+    <row r="70" spans="1:12">
       <c r="A70" t="s">
         <v>70</v>
       </c>
@@ -2221,8 +2982,19 @@
         <f>Table6[[#This Row],[max (mm)]]-Table6[[#This Row],[min (mm)]]</f>
         <v>245.32940000000002</v>
       </c>
-    </row>
-    <row r="72" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="I70" s="39" t="s">
+        <v>139</v>
+      </c>
+      <c r="J70" s="40"/>
+      <c r="K70" s="40"/>
+      <c r="L70" s="40"/>
+    </row>
+    <row r="71" spans="1:12">
+      <c r="J71" s="42" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="72" spans="1:12">
       <c r="A72" t="s">
         <v>27</v>
       </c>
@@ -2236,227 +3008,307 @@
         <v>24</v>
       </c>
     </row>
-    <row r="73" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:12">
       <c r="A73">
         <v>1</v>
       </c>
-      <c r="B73" s="6"/>
-      <c r="C73" s="2"/>
+      <c r="B73" s="6">
+        <v>7.6024000000000003</v>
+      </c>
+      <c r="C73" s="2">
+        <v>557.6</v>
+      </c>
       <c r="D73">
         <f>Table7[[#This Row],[max (mm)]]-Table7[[#This Row],[min (mm)]]</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="74" spans="1:4" x14ac:dyDescent="0.25">
+        <v>549.99760000000003</v>
+      </c>
+    </row>
+    <row r="74" spans="1:12">
       <c r="A74">
         <v>2</v>
       </c>
-      <c r="B74" s="6"/>
-      <c r="C74" s="2"/>
+      <c r="B74" s="6">
+        <v>6.5853000000000002</v>
+      </c>
+      <c r="C74" s="2">
+        <v>559.91</v>
+      </c>
       <c r="D74">
         <f>Table7[[#This Row],[max (mm)]]-Table7[[#This Row],[min (mm)]]</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="75" spans="1:4" x14ac:dyDescent="0.25">
+        <v>553.32470000000001</v>
+      </c>
+    </row>
+    <row r="75" spans="1:12">
       <c r="A75">
         <v>3</v>
       </c>
-      <c r="B75" s="6"/>
-      <c r="C75" s="2"/>
+      <c r="B75" s="6">
+        <v>6.585</v>
+      </c>
+      <c r="C75" s="2">
+        <v>559.91</v>
+      </c>
       <c r="D75">
         <f>Table7[[#This Row],[max (mm)]]-Table7[[#This Row],[min (mm)]]</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="76" spans="1:4" x14ac:dyDescent="0.25">
+        <v>553.32499999999993</v>
+      </c>
+    </row>
+    <row r="76" spans="1:12">
       <c r="A76">
         <v>4</v>
       </c>
-      <c r="B76" s="6"/>
-      <c r="C76" s="2"/>
+      <c r="B76" s="6">
+        <v>6.585</v>
+      </c>
+      <c r="C76" s="2">
+        <v>576.64</v>
+      </c>
       <c r="D76">
         <f>Table7[[#This Row],[max (mm)]]-Table7[[#This Row],[min (mm)]]</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="77" spans="1:4" x14ac:dyDescent="0.25">
+        <v>570.05499999999995</v>
+      </c>
+    </row>
+    <row r="77" spans="1:12">
       <c r="A77">
         <v>5</v>
       </c>
-      <c r="B77" s="6"/>
-      <c r="C77" s="2"/>
+      <c r="B77" s="6">
+        <v>6.585</v>
+      </c>
+      <c r="C77" s="2">
+        <v>576.64</v>
+      </c>
       <c r="D77">
         <f>Table7[[#This Row],[max (mm)]]-Table7[[#This Row],[min (mm)]]</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="78" spans="1:4" x14ac:dyDescent="0.25">
+        <v>570.05499999999995</v>
+      </c>
+    </row>
+    <row r="78" spans="1:12">
       <c r="A78">
         <v>6</v>
       </c>
-      <c r="B78" s="6"/>
-      <c r="C78" s="2"/>
+      <c r="B78" s="6">
+        <v>-1149</v>
+      </c>
+      <c r="C78" s="2">
+        <v>-9.6547000000000001</v>
+      </c>
       <c r="D78">
         <f>Table7[[#This Row],[max (mm)]]-Table7[[#This Row],[min (mm)]]</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="79" spans="1:4" x14ac:dyDescent="0.25">
+        <v>1139.3453</v>
+      </c>
+    </row>
+    <row r="79" spans="1:12">
       <c r="A79">
         <v>7</v>
       </c>
-      <c r="B79" s="6"/>
-      <c r="C79" s="2"/>
+      <c r="B79" s="6">
+        <v>33.917999999999999</v>
+      </c>
+      <c r="C79" s="2">
+        <v>311.38</v>
+      </c>
       <c r="D79">
         <f>Table7[[#This Row],[max (mm)]]-Table7[[#This Row],[min (mm)]]</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="80" spans="1:4" x14ac:dyDescent="0.25">
+        <v>277.46199999999999</v>
+      </c>
+    </row>
+    <row r="80" spans="1:12">
       <c r="A80">
         <v>8</v>
       </c>
-      <c r="B80" s="6"/>
-      <c r="C80" s="2"/>
+      <c r="B80" s="6">
+        <v>-14.363</v>
+      </c>
+      <c r="C80" s="2">
+        <v>310.5</v>
+      </c>
       <c r="D80">
         <f>Table7[[#This Row],[max (mm)]]-Table7[[#This Row],[min (mm)]]</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="81" spans="1:4" x14ac:dyDescent="0.25">
+        <v>324.863</v>
+      </c>
+    </row>
+    <row r="81" spans="1:4">
       <c r="A81">
         <v>9</v>
       </c>
-      <c r="B81" s="6"/>
-      <c r="C81" s="2"/>
+      <c r="B81" s="6">
+        <v>18.079999999999998</v>
+      </c>
+      <c r="C81" s="2">
+        <v>429.14</v>
+      </c>
       <c r="D81">
         <f>Table7[[#This Row],[max (mm)]]-Table7[[#This Row],[min (mm)]]</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="82" spans="1:4" x14ac:dyDescent="0.25">
+        <v>411.06</v>
+      </c>
+    </row>
+    <row r="82" spans="1:4">
       <c r="A82">
         <v>10</v>
       </c>
-      <c r="B82" s="6"/>
-      <c r="C82" s="2"/>
+      <c r="B82" s="6">
+        <v>-11.029</v>
+      </c>
+      <c r="C82" s="2">
+        <v>605.14</v>
+      </c>
       <c r="D82">
         <f>Table7[[#This Row],[max (mm)]]-Table7[[#This Row],[min (mm)]]</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="83" spans="1:4" x14ac:dyDescent="0.25">
+        <v>616.16899999999998</v>
+      </c>
+    </row>
+    <row r="83" spans="1:4">
       <c r="A83">
         <v>11</v>
       </c>
-      <c r="B83" s="6"/>
-      <c r="C83" s="2"/>
+      <c r="B83" s="6">
+        <v>924544</v>
+      </c>
+      <c r="C83" s="2">
+        <v>934324</v>
+      </c>
       <c r="D83">
         <f>Table7[[#This Row],[max (mm)]]-Table7[[#This Row],[min (mm)]]</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="84" spans="1:4" x14ac:dyDescent="0.25">
+        <v>9780</v>
+      </c>
+    </row>
+    <row r="84" spans="1:4">
       <c r="A84">
         <v>12</v>
       </c>
-      <c r="B84" s="6"/>
-      <c r="C84" s="2"/>
+      <c r="B84" s="6">
+        <v>923177</v>
+      </c>
+      <c r="C84" s="2">
+        <v>934554</v>
+      </c>
       <c r="D84">
         <f>Table7[[#This Row],[max (mm)]]-Table7[[#This Row],[min (mm)]]</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="85" spans="1:4" x14ac:dyDescent="0.25">
+        <v>11377</v>
+      </c>
+    </row>
+    <row r="85" spans="1:4">
       <c r="A85">
         <v>13</v>
       </c>
-      <c r="B85" s="6"/>
-      <c r="C85" s="2"/>
+      <c r="B85" s="6">
+        <v>597.16</v>
+      </c>
+      <c r="C85" s="2">
+        <v>317.81</v>
+      </c>
       <c r="D85">
         <f>Table7[[#This Row],[max (mm)]]-Table7[[#This Row],[min (mm)]]</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="86" spans="1:4" x14ac:dyDescent="0.25">
+        <v>-279.34999999999997</v>
+      </c>
+    </row>
+    <row r="86" spans="1:4">
       <c r="A86">
         <v>14</v>
       </c>
-      <c r="B86" s="6"/>
-      <c r="C86" s="2"/>
+      <c r="B86" s="6">
+        <v>598.79999999999995</v>
+      </c>
+      <c r="C86" s="2">
+        <v>328.98</v>
+      </c>
       <c r="D86">
         <f>Table7[[#This Row],[max (mm)]]-Table7[[#This Row],[min (mm)]]</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="87" spans="1:4" x14ac:dyDescent="0.25">
+        <v>-269.81999999999994</v>
+      </c>
+    </row>
+    <row r="87" spans="1:4">
       <c r="A87">
         <v>15</v>
       </c>
-      <c r="B87" s="6"/>
-      <c r="C87" s="2"/>
+      <c r="B87" s="6">
+        <v>147.85</v>
+      </c>
+      <c r="C87" s="2">
+        <v>502</v>
+      </c>
       <c r="D87">
         <f>Table7[[#This Row],[max (mm)]]-Table7[[#This Row],[min (mm)]]</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="88" spans="1:4" x14ac:dyDescent="0.25">
+        <v>354.15</v>
+      </c>
+    </row>
+    <row r="88" spans="1:4">
       <c r="A88">
         <v>16</v>
       </c>
-      <c r="B88" s="6"/>
-      <c r="C88" s="2"/>
+      <c r="B88" s="6">
+        <v>348.07</v>
+      </c>
+      <c r="C88" s="2">
+        <v>821.09</v>
+      </c>
       <c r="D88">
         <f>Table7[[#This Row],[max (mm)]]-Table7[[#This Row],[min (mm)]]</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="89" spans="1:4" x14ac:dyDescent="0.25">
+        <v>473.02000000000004</v>
+      </c>
+    </row>
+    <row r="89" spans="1:4">
       <c r="A89">
         <v>17</v>
       </c>
-      <c r="B89" s="6"/>
-      <c r="C89" s="2"/>
+      <c r="B89" s="6">
+        <v>17.748000000000001</v>
+      </c>
+      <c r="C89" s="2">
+        <v>684.41</v>
+      </c>
       <c r="D89">
         <f>Table7[[#This Row],[max (mm)]]-Table7[[#This Row],[min (mm)]]</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="90" spans="1:4" x14ac:dyDescent="0.25">
+        <v>666.66199999999992</v>
+      </c>
+    </row>
+    <row r="90" spans="1:4">
       <c r="A90">
         <v>18</v>
       </c>
-      <c r="B90" s="6"/>
-      <c r="C90" s="2"/>
+      <c r="B90" s="6">
+        <v>-155.75</v>
+      </c>
+      <c r="C90" s="2">
+        <v>248.88</v>
+      </c>
       <c r="D90">
         <f>Table7[[#This Row],[max (mm)]]-Table7[[#This Row],[min (mm)]]</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="91" spans="1:4" x14ac:dyDescent="0.25">
+        <v>404.63</v>
+      </c>
+    </row>
+    <row r="91" spans="1:4">
       <c r="A91">
         <v>19</v>
       </c>
-      <c r="B91" s="6"/>
-      <c r="C91" s="2"/>
+      <c r="B91" s="6">
+        <v>449.47</v>
+      </c>
+      <c r="C91" s="2">
+        <v>370.54</v>
+      </c>
       <c r="D91">
         <f>Table7[[#This Row],[max (mm)]]-Table7[[#This Row],[min (mm)]]</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="92" spans="1:4" x14ac:dyDescent="0.25">
+        <v>-78.930000000000007</v>
+      </c>
+    </row>
+    <row r="92" spans="1:4">
       <c r="A92">
         <v>20</v>
       </c>
-      <c r="B92" s="6"/>
-      <c r="C92" s="2"/>
+      <c r="B92" s="6">
+        <v>-34.231000000000002</v>
+      </c>
+      <c r="C92" s="2">
+        <v>482.67</v>
+      </c>
       <c r="D92">
         <f>Table7[[#This Row],[max (mm)]]-Table7[[#This Row],[min (mm)]]</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="94" spans="1:4" x14ac:dyDescent="0.25">
+        <v>516.90100000000007</v>
+      </c>
+    </row>
+    <row r="94" spans="1:4">
       <c r="A94" t="s">
         <v>28</v>
       </c>
@@ -2470,7 +3322,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="95" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:4">
       <c r="A95">
         <v>1</v>
       </c>
@@ -2481,7 +3333,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="96" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:4">
       <c r="A96">
         <v>2</v>
       </c>
@@ -2492,7 +3344,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="97" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:4">
       <c r="A97">
         <v>3</v>
       </c>
@@ -2503,7 +3355,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="98" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:4">
       <c r="A98">
         <v>4</v>
       </c>
@@ -2514,7 +3366,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="99" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:4">
       <c r="A99">
         <v>5</v>
       </c>
@@ -2525,7 +3377,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="100" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:4">
       <c r="A100">
         <v>6</v>
       </c>
@@ -2536,7 +3388,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="101" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:4">
       <c r="A101">
         <v>7</v>
       </c>
@@ -2547,7 +3399,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="102" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:4">
       <c r="A102">
         <v>8</v>
       </c>
@@ -2558,7 +3410,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="103" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="103" spans="1:4">
       <c r="A103">
         <v>9</v>
       </c>
@@ -2569,7 +3421,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="104" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="104" spans="1:4">
       <c r="A104">
         <v>10</v>
       </c>
@@ -2580,7 +3432,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="105" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="105" spans="1:4">
       <c r="A105">
         <v>11</v>
       </c>
@@ -2591,7 +3443,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="106" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="106" spans="1:4">
       <c r="A106">
         <v>12</v>
       </c>
@@ -2602,7 +3454,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="107" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="107" spans="1:4">
       <c r="A107">
         <v>13</v>
       </c>
@@ -2613,7 +3465,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="108" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="108" spans="1:4">
       <c r="A108">
         <v>14</v>
       </c>
@@ -2624,7 +3476,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="109" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="109" spans="1:4">
       <c r="A109">
         <v>15</v>
       </c>
@@ -2635,7 +3487,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="110" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="110" spans="1:4">
       <c r="A110">
         <v>16</v>
       </c>
@@ -2646,7 +3498,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="111" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="111" spans="1:4">
       <c r="A111">
         <v>17</v>
       </c>
@@ -2657,7 +3509,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="112" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="112" spans="1:4">
       <c r="A112">
         <v>18</v>
       </c>
@@ -2668,7 +3520,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="113" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="113" spans="1:4">
       <c r="A113">
         <v>19</v>
       </c>
@@ -2679,7 +3531,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="114" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="114" spans="1:4">
       <c r="A114">
         <v>20</v>
       </c>

</xml_diff>

<commit_message>
aligning min depth to screen - objects
</commit_message>
<xml_diff>
--- a/Stimuli/Images/DepthMaps/depths.xlsx
+++ b/Stimuli/Images/DepthMaps/depths.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Becca\Documents\GitHub\fMRI_ef_scrambled-objects_2022\Stimuli\Images\DepthMaps\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C8A70D01-18D0-4CCE-84FB-6337008122B8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CBA0CF35-1CA6-4A68-8DE0-4562A414AEAB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{A60B6263-5EC6-4E52-B93A-1BC494533CA5}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{A60B6263-5EC6-4E52-B93A-1BC494533CA5}"/>
   </bookViews>
   <sheets>
     <sheet name="histogram" sheetId="4" r:id="rId1"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="388" uniqueCount="174">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="389" uniqueCount="175">
   <si>
     <t>apple</t>
   </si>
@@ -583,6 +583,9 @@
   </si>
   <si>
     <t>object-solid_18</t>
+  </si>
+  <si>
+    <t>mean</t>
   </si>
 </sst>
 </file>
@@ -2269,7 +2272,9 @@
     <tableColumn id="7" xr3:uid="{5C947B0D-2C2B-4626-A556-1DFD4728AEBA}" name="ID" dataDxfId="5"/>
     <tableColumn id="2" xr3:uid="{B62FA381-A946-4C5D-87B0-25C94F47947E}" name="min (mm)" dataDxfId="4"/>
     <tableColumn id="3" xr3:uid="{E5755554-E1B0-494A-92FB-875744A3C7EC}" name="max (mm)" dataDxfId="3"/>
-    <tableColumn id="4" xr3:uid="{146B5C7C-63AD-4333-A553-A05D927737AB}" name="difference (mm)" dataDxfId="2"/>
+    <tableColumn id="4" xr3:uid="{146B5C7C-63AD-4333-A553-A05D927737AB}" name="difference (mm)" dataDxfId="2">
+      <calculatedColumnFormula>Table9[[#This Row],[max (mm)]]-Table9[[#This Row],[min (mm)]]</calculatedColumnFormula>
+    </tableColumn>
     <tableColumn id="5" xr3:uid="{02D3617A-3D9C-4CA4-9AB7-E7F68D9DF901}" name="visible max" dataDxfId="1"/>
     <tableColumn id="6" xr3:uid="{EC7B00FC-44A9-4F2E-97B8-AD1785358F4A}" name="visible range" dataDxfId="0">
       <calculatedColumnFormula>F3-C3</calculatedColumnFormula>
@@ -2744,7 +2749,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9D578D86-D93F-4507-92E5-98F2DF597463}">
   <dimension ref="A1:BA16"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C3" sqref="C3:BA16"/>
     </sheetView>
   </sheetViews>
@@ -5216,10 +5221,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EEAEED5E-03E1-4D43-B753-B6D0E922BAC9}">
-  <dimension ref="A2:H79"/>
+  <dimension ref="A2:I79"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="G11" sqref="G11"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B13" sqref="B13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -5232,7 +5237,7 @@
     <col min="6" max="7" width="14.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:7" ht="15.75" thickBot="1">
+    <row r="2" spans="1:9" ht="15.75" thickBot="1">
       <c r="A2" s="38" t="s">
         <v>25</v>
       </c>
@@ -5254,8 +5259,15 @@
       <c r="G2" s="41" t="s">
         <v>146</v>
       </c>
-    </row>
-    <row r="3" spans="1:7" ht="15.75" thickTop="1">
+      <c r="H2" t="s">
+        <v>174</v>
+      </c>
+      <c r="I2">
+        <f>AVERAGE(Table9[visible range])</f>
+        <v>136.06099999999998</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" ht="15.75" thickTop="1">
       <c r="A3" s="31" t="s">
         <v>1</v>
       </c>
@@ -5263,24 +5275,24 @@
         <v>94</v>
       </c>
       <c r="C3" s="32">
-        <v>-0.90100000000000002</v>
+        <v>0</v>
       </c>
       <c r="D3" s="33">
-        <v>194.2</v>
+        <v>195.12</v>
       </c>
       <c r="E3" s="33">
-        <f>final!$D4-final!$C4</f>
-        <v>175.81800000000001</v>
+        <f>Table9[[#This Row],[max (mm)]]-Table9[[#This Row],[min (mm)]]</f>
+        <v>195.12</v>
       </c>
       <c r="F3" s="31">
         <v>179.68</v>
       </c>
       <c r="G3" s="30">
-        <f t="shared" ref="G3:G15" si="0">F3-C3</f>
-        <v>180.58100000000002</v>
-      </c>
-    </row>
-    <row r="4" spans="1:7">
+        <f>F3-C3</f>
+        <v>179.68</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9">
       <c r="A4" s="31" t="s">
         <v>2</v>
       </c>
@@ -5288,24 +5300,24 @@
         <v>95</v>
       </c>
       <c r="C4" s="32">
-        <v>-0.19800000000000001</v>
+        <v>0</v>
       </c>
       <c r="D4" s="33">
-        <v>175.62</v>
+        <v>175.82</v>
       </c>
       <c r="E4" s="33">
-        <f>final!$D5-final!$C5</f>
-        <v>181.755</v>
+        <f>Table9[[#This Row],[max (mm)]]-Table9[[#This Row],[min (mm)]]</f>
+        <v>175.82</v>
       </c>
       <c r="F4" s="31">
         <v>157.1</v>
       </c>
       <c r="G4" s="30">
-        <f t="shared" si="0"/>
-        <v>157.298</v>
-      </c>
-    </row>
-    <row r="5" spans="1:7">
+        <f>F4-C4</f>
+        <v>157.1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9">
       <c r="A5" s="31" t="s">
         <v>3</v>
       </c>
@@ -5313,24 +5325,24 @@
         <v>96</v>
       </c>
       <c r="C5" s="32">
-        <v>1.345</v>
+        <v>0</v>
       </c>
       <c r="D5" s="33">
-        <v>183.1</v>
+        <v>181.751</v>
       </c>
       <c r="E5" s="33">
-        <f>final!$D6-final!$C6</f>
-        <v>244.828</v>
+        <f>Table9[[#This Row],[max (mm)]]-Table9[[#This Row],[min (mm)]]</f>
+        <v>181.751</v>
       </c>
       <c r="F5" s="31">
         <v>103.26</v>
       </c>
       <c r="G5" s="30">
-        <f t="shared" si="0"/>
-        <v>101.91500000000001</v>
-      </c>
-    </row>
-    <row r="6" spans="1:7">
+        <f>F5-C5</f>
+        <v>103.26</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9">
       <c r="A6" s="31" t="s">
         <v>4</v>
       </c>
@@ -5338,24 +5350,24 @@
         <v>97</v>
       </c>
       <c r="C6" s="32">
-        <v>0.65200000000000002</v>
+        <v>0</v>
       </c>
       <c r="D6" s="33">
-        <v>245.48</v>
+        <v>145.874</v>
       </c>
       <c r="E6" s="33">
-        <f>final!$D7-final!$C7</f>
-        <v>144.29129999999998</v>
+        <f>Table9[[#This Row],[max (mm)]]-Table9[[#This Row],[min (mm)]]</f>
+        <v>145.874</v>
       </c>
       <c r="F6" s="31">
-        <v>186.46</v>
+        <v>128.85</v>
       </c>
       <c r="G6" s="30">
-        <f t="shared" si="0"/>
-        <v>185.80800000000002</v>
-      </c>
-    </row>
-    <row r="7" spans="1:7">
+        <f>F6-C6</f>
+        <v>128.85</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9">
       <c r="A7" s="31" t="s">
         <v>5</v>
       </c>
@@ -5363,24 +5375,24 @@
         <v>98</v>
       </c>
       <c r="C7" s="32">
-        <v>-1.2813000000000001</v>
+        <v>0</v>
       </c>
       <c r="D7" s="33">
-        <v>143.01</v>
+        <v>144.76</v>
       </c>
       <c r="E7" s="33">
-        <f>final!$D8-final!$C8</f>
-        <v>192.851</v>
+        <f>Table9[[#This Row],[max (mm)]]-Table9[[#This Row],[min (mm)]]</f>
+        <v>144.76</v>
       </c>
       <c r="F7" s="31">
         <v>113</v>
       </c>
       <c r="G7" s="30">
-        <f t="shared" si="0"/>
-        <v>114.2813</v>
-      </c>
-    </row>
-    <row r="8" spans="1:7">
+        <f>F7-C7</f>
+        <v>113</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9">
       <c r="A8" s="31" t="s">
         <v>0</v>
       </c>
@@ -5388,24 +5400,24 @@
         <v>93</v>
       </c>
       <c r="C8" s="32">
-        <v>3.5190000000000001</v>
+        <v>0</v>
       </c>
       <c r="D8" s="33">
-        <v>196.37</v>
+        <v>192.85</v>
       </c>
       <c r="E8" s="33">
-        <f>final!$D3-final!$C3</f>
-        <v>195.101</v>
+        <f>Table9[[#This Row],[max (mm)]]-Table9[[#This Row],[min (mm)]]</f>
+        <v>192.85</v>
       </c>
       <c r="F8" s="31">
         <v>124.35</v>
       </c>
       <c r="G8" s="30">
-        <f t="shared" si="0"/>
-        <v>120.83099999999999</v>
-      </c>
-    </row>
-    <row r="9" spans="1:7">
+        <f>F8-C8</f>
+        <v>124.35</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9">
       <c r="A9" s="31" t="s">
         <v>6</v>
       </c>
@@ -5413,23 +5425,24 @@
         <v>99</v>
       </c>
       <c r="C9" s="32">
-        <v>0.11887</v>
+        <v>0</v>
       </c>
       <c r="D9" s="33">
-        <v>154.1</v>
+        <v>154.18</v>
       </c>
       <c r="E9" s="33">
-        <v>115.7158</v>
+        <f>Table9[[#This Row],[max (mm)]]-Table9[[#This Row],[min (mm)]]</f>
+        <v>154.18</v>
       </c>
       <c r="F9" s="31">
         <v>128.87</v>
       </c>
       <c r="G9" s="30">
-        <f t="shared" si="0"/>
-        <v>128.75113000000002</v>
-      </c>
-    </row>
-    <row r="10" spans="1:7">
+        <f>F9-C9</f>
+        <v>128.87</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9">
       <c r="A10" s="31" t="s">
         <v>143</v>
       </c>
@@ -5437,23 +5450,24 @@
         <v>100</v>
       </c>
       <c r="C10" s="32">
-        <v>1.0669</v>
+        <v>0</v>
       </c>
       <c r="D10" s="33">
-        <v>110.64</v>
+        <v>113.92</v>
       </c>
       <c r="E10" s="33">
-        <v>109.5731</v>
+        <f>Table9[[#This Row],[max (mm)]]-Table9[[#This Row],[min (mm)]]</f>
+        <v>113.92</v>
       </c>
       <c r="F10" s="31">
-        <v>206.13</v>
+        <v>112.93</v>
       </c>
       <c r="G10" s="30">
-        <f t="shared" si="0"/>
-        <v>205.06309999999999</v>
-      </c>
-    </row>
-    <row r="11" spans="1:7">
+        <f>F10-C10</f>
+        <v>112.93</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9">
       <c r="A11" s="31" t="s">
         <v>10</v>
       </c>
@@ -5461,24 +5475,24 @@
         <v>102</v>
       </c>
       <c r="C11" s="32">
-        <v>-1.1919</v>
+        <v>0</v>
       </c>
       <c r="D11" s="33">
-        <v>165.73</v>
+        <v>166.92500000000001</v>
       </c>
       <c r="E11" s="33">
-        <f>final!$D10-final!$C10</f>
-        <v>109.5731</v>
+        <f>Table9[[#This Row],[max (mm)]]-Table9[[#This Row],[min (mm)]]</f>
+        <v>166.92500000000001</v>
       </c>
       <c r="F11" s="31">
         <v>113.06</v>
       </c>
       <c r="G11" s="30">
-        <f t="shared" si="0"/>
-        <v>114.25190000000001</v>
-      </c>
-    </row>
-    <row r="12" spans="1:7">
+        <f>F11-C11</f>
+        <v>113.06</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9">
       <c r="A12" s="31" t="s">
         <v>11</v>
       </c>
@@ -5486,24 +5500,24 @@
         <v>103</v>
       </c>
       <c r="C12" s="32">
-        <v>1.0129999999999999</v>
+        <v>0</v>
       </c>
       <c r="D12" s="33">
-        <v>216.27</v>
+        <v>215.63900000000001</v>
       </c>
       <c r="E12" s="33">
-        <f>final!$D11-final!$C11</f>
-        <v>166.92189999999999</v>
+        <f>Table9[[#This Row],[max (mm)]]-Table9[[#This Row],[min (mm)]]</f>
+        <v>215.63900000000001</v>
       </c>
       <c r="F12" s="31">
         <v>212.12</v>
       </c>
       <c r="G12" s="30">
-        <f t="shared" si="0"/>
-        <v>211.107</v>
-      </c>
-    </row>
-    <row r="13" spans="1:7">
+        <f>F12-C12</f>
+        <v>212.12</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9">
       <c r="A13" s="31" t="s">
         <v>15</v>
       </c>
@@ -5511,23 +5525,24 @@
         <v>105</v>
       </c>
       <c r="C13" s="32">
-        <v>7.79</v>
+        <v>0</v>
       </c>
       <c r="D13" s="33">
-        <v>131.26</v>
+        <v>168.446</v>
       </c>
       <c r="E13" s="33">
-        <v>123.47</v>
+        <f>Table9[[#This Row],[max (mm)]]-Table9[[#This Row],[min (mm)]]</f>
+        <v>168.446</v>
       </c>
       <c r="F13" s="31">
-        <v>112.9</v>
+        <v>166.15100000000001</v>
       </c>
       <c r="G13" s="30">
-        <f t="shared" si="0"/>
-        <v>105.11</v>
-      </c>
-    </row>
-    <row r="14" spans="1:7">
+        <f>F13-C13</f>
+        <v>166.15100000000001</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9">
       <c r="A14" s="31" t="s">
         <v>17</v>
       </c>
@@ -5535,24 +5550,24 @@
         <v>173</v>
       </c>
       <c r="C14" s="32">
-        <v>2.6749999999999998</v>
+        <v>0</v>
       </c>
       <c r="D14" s="33">
-        <v>185.83</v>
+        <v>183.06700000000001</v>
       </c>
       <c r="E14" s="33">
-        <f>final!$D14-final!$C14</f>
-        <v>183.155</v>
+        <f>Table9[[#This Row],[max (mm)]]-Table9[[#This Row],[min (mm)]]</f>
+        <v>183.06700000000001</v>
       </c>
       <c r="F14" s="31">
         <v>169.43</v>
       </c>
       <c r="G14" s="30">
-        <f t="shared" si="0"/>
-        <v>166.755</v>
-      </c>
-    </row>
-    <row r="15" spans="1:7">
+        <f>F14-C14</f>
+        <v>169.43</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9">
       <c r="A15" s="34" t="s">
         <v>18</v>
       </c>
@@ -5560,24 +5575,24 @@
         <v>104</v>
       </c>
       <c r="C15" s="35">
-        <v>1.5624</v>
+        <v>0</v>
       </c>
       <c r="D15" s="36">
-        <v>75.668999999999997</v>
-      </c>
-      <c r="E15" s="36">
-        <f>final!$D15-final!$C15</f>
-        <v>74.1066</v>
+        <v>132.87200000000001</v>
+      </c>
+      <c r="E15" s="33">
+        <f>Table9[[#This Row],[max (mm)]]-Table9[[#This Row],[min (mm)]]</f>
+        <v>132.87200000000001</v>
       </c>
       <c r="F15" s="34">
         <v>59.991999999999997</v>
       </c>
       <c r="G15" s="30">
-        <f t="shared" si="0"/>
-        <v>58.429600000000001</v>
-      </c>
-    </row>
-    <row r="16" spans="1:7">
+        <f>F15-C15</f>
+        <v>59.991999999999997</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9">
       <c r="A16" s="30"/>
       <c r="B16" s="30"/>
       <c r="C16" s="30"/>
@@ -5586,7 +5601,7 @@
       <c r="F16" s="30"/>
       <c r="G16" s="30"/>
     </row>
-    <row r="17" spans="1:7" ht="15.75" thickBot="1">
+    <row r="17" spans="1:9" ht="15.75" thickBot="1">
       <c r="A17" s="37" t="s">
         <v>91</v>
       </c>
@@ -5608,8 +5623,12 @@
       <c r="G17" s="37" t="s">
         <v>146</v>
       </c>
-    </row>
-    <row r="18" spans="1:7" ht="15.75" thickTop="1">
+      <c r="I17">
+        <f>AVERAGE(Table2[visible range])</f>
+        <v>115.71791647058822</v>
+      </c>
+    </row>
+    <row r="18" spans="1:9" ht="15.75" thickTop="1">
       <c r="A18" s="30" t="s">
         <v>33</v>
       </c>
@@ -5623,7 +5642,7 @@
         <v>107.57</v>
       </c>
       <c r="E18" s="31">
-        <f t="shared" ref="E18:E34" si="1">D18-C18</f>
+        <f t="shared" ref="E18:E34" si="0">D18-C18</f>
         <v>88.768000000000001</v>
       </c>
       <c r="F18" s="31">
@@ -5634,7 +5653,7 @@
         <v>81.298000000000002</v>
       </c>
     </row>
-    <row r="19" spans="1:7">
+    <row r="19" spans="1:9">
       <c r="A19" s="30" t="s">
         <v>32</v>
       </c>
@@ -5648,7 +5667,7 @@
         <v>63.771000000000001</v>
       </c>
       <c r="E19" s="31">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>65.040900000000008</v>
       </c>
       <c r="F19" s="31">
@@ -5659,7 +5678,7 @@
         <v>51.322899999999997</v>
       </c>
     </row>
-    <row r="20" spans="1:7">
+    <row r="20" spans="1:9">
       <c r="A20" s="30" t="s">
         <v>31</v>
       </c>
@@ -5673,7 +5692,7 @@
         <v>149.52000000000001</v>
       </c>
       <c r="E20" s="31">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>150.31393</v>
       </c>
       <c r="F20" s="31">
@@ -5684,7 +5703,7 @@
         <v>125.21393</v>
       </c>
     </row>
-    <row r="21" spans="1:7">
+    <row r="21" spans="1:9">
       <c r="A21" s="30" t="s">
         <v>30</v>
       </c>
@@ -5692,24 +5711,24 @@
         <v>75</v>
       </c>
       <c r="C21" s="32">
-        <v>-4.0918999999999999</v>
+        <v>0</v>
       </c>
       <c r="D21" s="33">
-        <v>128.72</v>
+        <v>132.83000000000001</v>
       </c>
       <c r="E21" s="31">
-        <f t="shared" si="1"/>
-        <v>132.81190000000001</v>
+        <f t="shared" si="0"/>
+        <v>132.83000000000001</v>
       </c>
       <c r="F21" s="31">
-        <v>103.06</v>
+        <v>101.886</v>
       </c>
       <c r="G21" s="33">
         <f>Table2[[#This Row],[visible max]]-Table2[[#This Row],[min (mm)]]</f>
-        <v>107.1519</v>
-      </c>
-    </row>
-    <row r="22" spans="1:7">
+        <v>101.886</v>
+      </c>
+    </row>
+    <row r="22" spans="1:9">
       <c r="A22" s="30" t="s">
         <v>29</v>
       </c>
@@ -5723,7 +5742,7 @@
         <v>107.87</v>
       </c>
       <c r="E22" s="31">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>106.622</v>
       </c>
       <c r="F22" s="31">
@@ -5734,7 +5753,7 @@
         <v>88.481999999999999</v>
       </c>
     </row>
-    <row r="23" spans="1:7">
+    <row r="23" spans="1:9">
       <c r="A23" s="30" t="s">
         <v>34</v>
       </c>
@@ -5748,7 +5767,7 @@
         <v>145.69</v>
       </c>
       <c r="E23" s="31">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>154.93279999999999</v>
       </c>
       <c r="F23" s="31">
@@ -5759,7 +5778,7 @@
         <v>100.0128</v>
       </c>
     </row>
-    <row r="24" spans="1:7">
+    <row r="24" spans="1:9">
       <c r="A24" s="30" t="s">
         <v>35</v>
       </c>
@@ -5773,7 +5792,7 @@
         <v>204.01</v>
       </c>
       <c r="E24" s="31">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>208.56829999999999</v>
       </c>
       <c r="F24" s="31">
@@ -5784,7 +5803,7 @@
         <v>189.63830000000002</v>
       </c>
     </row>
-    <row r="25" spans="1:7">
+    <row r="25" spans="1:9">
       <c r="A25" s="30" t="s">
         <v>36</v>
       </c>
@@ -5798,7 +5817,7 @@
         <v>118.52</v>
       </c>
       <c r="E25" s="31">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>121.0046</v>
       </c>
       <c r="F25" s="31">
@@ -5809,7 +5828,7 @@
         <v>105.49460000000001</v>
       </c>
     </row>
-    <row r="26" spans="1:7">
+    <row r="26" spans="1:9">
       <c r="A26" s="30" t="s">
         <v>37</v>
       </c>
@@ -5823,7 +5842,7 @@
         <v>146.65</v>
       </c>
       <c r="E26" s="31">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>145.59620000000001</v>
       </c>
       <c r="F26" s="31">
@@ -5834,7 +5853,7 @@
         <v>126.53620000000001</v>
       </c>
     </row>
-    <row r="27" spans="1:7">
+    <row r="27" spans="1:9">
       <c r="A27" s="30" t="s">
         <v>38</v>
       </c>
@@ -5848,7 +5867,7 @@
         <v>122.57</v>
       </c>
       <c r="E27" s="31">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>121.78063999999999</v>
       </c>
       <c r="F27" s="31">
@@ -5859,7 +5878,7 @@
         <v>104.96064</v>
       </c>
     </row>
-    <row r="28" spans="1:7">
+    <row r="28" spans="1:9">
       <c r="A28" s="30" t="s">
         <v>39</v>
       </c>
@@ -5873,7 +5892,7 @@
         <v>195.61</v>
       </c>
       <c r="E28" s="31">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>180.04400000000001</v>
       </c>
       <c r="F28" s="31">
@@ -5884,7 +5903,7 @@
         <v>145.41399999999999</v>
       </c>
     </row>
-    <row r="29" spans="1:7">
+    <row r="29" spans="1:9">
       <c r="A29" s="30" t="s">
         <v>40</v>
       </c>
@@ -5898,7 +5917,7 @@
         <v>90.212999999999994</v>
       </c>
       <c r="E29" s="31">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>88.77579999999999</v>
       </c>
       <c r="F29" s="31">
@@ -5909,7 +5928,7 @@
         <v>59.876800000000003</v>
       </c>
     </row>
-    <row r="30" spans="1:7">
+    <row r="30" spans="1:9">
       <c r="A30" s="30" t="s">
         <v>41</v>
       </c>
@@ -5923,7 +5942,7 @@
         <v>194.42</v>
       </c>
       <c r="E30" s="31">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>200.54479999999998</v>
       </c>
       <c r="F30" s="31">
@@ -5934,7 +5953,7 @@
         <v>177.54479999999998</v>
       </c>
     </row>
-    <row r="31" spans="1:7">
+    <row r="31" spans="1:9">
       <c r="A31" s="30" t="s">
         <v>43</v>
       </c>
@@ -5948,7 +5967,7 @@
         <v>127.26</v>
       </c>
       <c r="E31" s="31">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>133.28919999999999</v>
       </c>
       <c r="F31" s="31">
@@ -5959,7 +5978,7 @@
         <v>119.7392</v>
       </c>
     </row>
-    <row r="32" spans="1:7">
+    <row r="32" spans="1:9">
       <c r="A32" s="30" t="s">
         <v>44</v>
       </c>
@@ -5973,7 +5992,7 @@
         <v>138.08000000000001</v>
       </c>
       <c r="E32" s="31">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>137.42746000000002</v>
       </c>
       <c r="F32" s="31">
@@ -5998,7 +6017,7 @@
         <v>201.68</v>
       </c>
       <c r="E33" s="31">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>200.94985</v>
       </c>
       <c r="F33" s="31">
@@ -6023,7 +6042,7 @@
         <v>146.99</v>
       </c>
       <c r="E34" s="31">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>145.4871</v>
       </c>
       <c r="F34" s="34">
@@ -6672,14 +6691,14 @@
         <v>177.65700000000001</v>
       </c>
       <c r="E62">
-        <f t="shared" ref="E62:E75" si="2">D62-C62</f>
+        <f t="shared" ref="E62:E75" si="1">D62-C62</f>
         <v>193.51400000000001</v>
       </c>
       <c r="F62" s="2">
         <v>177.65700000000001</v>
       </c>
       <c r="G62">
-        <f t="shared" ref="G62:G75" si="3">F62-C62</f>
+        <f t="shared" ref="G62:G75" si="2">F62-C62</f>
         <v>193.51400000000001</v>
       </c>
     </row>
@@ -6697,14 +6716,14 @@
         <v>311.38</v>
       </c>
       <c r="E63">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>277.46199999999999</v>
       </c>
       <c r="F63" s="2">
         <v>311.38</v>
       </c>
       <c r="G63">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>277.46199999999999</v>
       </c>
     </row>
@@ -6722,14 +6741,14 @@
         <v>310.5</v>
       </c>
       <c r="E64">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>324.863</v>
       </c>
       <c r="F64" s="2">
         <v>310.5</v>
       </c>
       <c r="G64">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>324.863</v>
       </c>
     </row>
@@ -6747,14 +6766,14 @@
         <v>429.14</v>
       </c>
       <c r="E65">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>411.06</v>
       </c>
       <c r="F65" s="2">
         <v>429.14</v>
       </c>
       <c r="G65">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>411.06</v>
       </c>
     </row>
@@ -6772,14 +6791,14 @@
         <v>605.14</v>
       </c>
       <c r="E66">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>616.16899999999998</v>
       </c>
       <c r="F66" s="2">
         <v>605.14</v>
       </c>
       <c r="G66">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>616.16899999999998</v>
       </c>
     </row>
@@ -6797,14 +6816,14 @@
         <v>934324</v>
       </c>
       <c r="E67">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>9780</v>
       </c>
       <c r="F67" s="2">
         <v>934324</v>
       </c>
       <c r="G67">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>9780</v>
       </c>
     </row>
@@ -6822,14 +6841,14 @@
         <v>934554</v>
       </c>
       <c r="E68">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>11377</v>
       </c>
       <c r="F68" s="2">
         <v>934554</v>
       </c>
       <c r="G68">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>11377</v>
       </c>
     </row>
@@ -6847,14 +6866,14 @@
         <v>597.16</v>
       </c>
       <c r="E69">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>279.34999999999997</v>
       </c>
       <c r="F69" s="2">
         <v>597.16</v>
       </c>
       <c r="G69">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>279.34999999999997</v>
       </c>
     </row>
@@ -6872,14 +6891,14 @@
         <v>598.79999999999995</v>
       </c>
       <c r="E70">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>269.81999999999994</v>
       </c>
       <c r="F70" s="2">
         <v>598.79999999999995</v>
       </c>
       <c r="G70">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>269.81999999999994</v>
       </c>
     </row>
@@ -6897,14 +6916,14 @@
         <v>502</v>
       </c>
       <c r="E71">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>354.15</v>
       </c>
       <c r="F71" s="2">
         <v>502</v>
       </c>
       <c r="G71">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>354.15</v>
       </c>
     </row>
@@ -6922,14 +6941,14 @@
         <v>821.09</v>
       </c>
       <c r="E72">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>473.02000000000004</v>
       </c>
       <c r="F72" s="2">
         <v>821.09</v>
       </c>
       <c r="G72">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>473.02000000000004</v>
       </c>
     </row>
@@ -6947,14 +6966,14 @@
         <v>684.41</v>
       </c>
       <c r="E73">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>666.66199999999992</v>
       </c>
       <c r="F73" s="2">
         <v>684.41</v>
       </c>
       <c r="G73">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>666.66199999999992</v>
       </c>
     </row>
@@ -6972,14 +6991,14 @@
         <v>248.88</v>
       </c>
       <c r="E74">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>404.63</v>
       </c>
       <c r="F74" s="2">
         <v>248.88</v>
       </c>
       <c r="G74">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>404.63</v>
       </c>
     </row>
@@ -6997,14 +7016,14 @@
         <v>482.67</v>
       </c>
       <c r="E75">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>516.90100000000007</v>
       </c>
       <c r="F75" s="2">
         <v>482.67</v>
       </c>
       <c r="G75">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>516.90100000000007</v>
       </c>
     </row>

</xml_diff>